<commit_message>
query find employee for report qpp007
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrken57/Work/UniversalK/project/export/qpp007/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrken57/Work/UniversalK/project/UniversalK/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$O$65</definedName>
     <definedName name="RangeChildRaising">Sheet1!#REF!</definedName>
     <definedName name="RangeChildRaisingManual">Sheet1!$A$6:$Q$6</definedName>
     <definedName name="RangeDeliveryNoticeAmount">Sheet1!#REF!</definedName>
@@ -117,14 +116,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,49 +448,49 @@
   <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C4"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="20.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.83203125" style="1"/>
-    <col min="2" max="16384" width="20.83203125" style="2"/>
+    <col min="1" max="1" width="16" style="1"/>
+    <col min="2" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="O5" s="7"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="O5" s="5"/>
     </row>
     <row r="6" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="O6" s="4"/>
@@ -514,7 +513,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="41" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L【日通システム株式会社】</oddHeader>
   </headerFooter>

</xml_diff>

<commit_message>
break page vertical for report qpp007
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrken57/Work/UniversalK/project/UniversalK/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nws_tiendd\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$216</definedName>
     <definedName name="RangeChildRaising">Sheet1!#REF!</definedName>
     <definedName name="RangeChildRaisingManual">Sheet1!$A$6:$Q$6</definedName>
     <definedName name="RangeDeliveryNoticeAmount">Sheet1!#REF!</definedName>
@@ -23,16 +24,13 @@
     <definedName name="RangeFooterEachOffice">Sheet1!#REF!</definedName>
     <definedName name="RangeOffice">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -104,26 +102,26 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,80 +445,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="62" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16" style="1"/>
+    <col min="1" max="1" width="26.7109375" style="7" customWidth="1"/>
     <col min="2" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:16" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:16" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="O5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
+    <row r="6" spans="1:16" s="5" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A1:B1"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A1:M1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="55" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="53" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L【日通システム株式会社】</oddHeader>
   </headerFooter>
-  <rowBreaks count="2" manualBreakCount="2">
-    <brk id="65" max="14" man="1"/>
-    <brk id="125" max="16" man="1"/>
-  </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Revert "Merge branch 'pr/pr.core/teame/kcp' into sys/develop"
This reverts commit 2551d4792da4d29ded719bca389a2e21d9433224, reversing
changes made to f92f3bd84a741ea379a9b5c63e87690319303dc2.
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP007.xlsx
@@ -1,36 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Server\wildfly-9.0.2.Final\standalone\deployments\nts.uk.pr.web.war\WEB-INF\lib\nts.uk.file.pr.infra.jar\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrken57/Work/UniversalK/project/UniversalK/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21135" windowWidth="38400" windowHeight="21135"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$M$134</definedName>
     <definedName name="RangeChildRaising">Sheet1!#REF!</definedName>
-    <definedName name="RangeChildRaisingManual">Sheet1!$A$7:$Q$7</definedName>
+    <definedName name="RangeChildRaisingManual">Sheet1!$A$6:$Q$6</definedName>
     <definedName name="RangeDeliveryNoticeAmount">Sheet1!#REF!</definedName>
     <definedName name="RangeDeliveryNoticeAmountManual">Sheet1!#REF!</definedName>
     <definedName name="RangeEmployee">Sheet1!#REF!</definedName>
     <definedName name="RangeFooterEachOffice">Sheet1!#REF!</definedName>
     <definedName name="RangeOffice">Sheet1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -58,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,16 +75,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="IPAPGothic"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="20"/>
       <color theme="1"/>
-      <name val="IPAPGothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -105,31 +102,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,104 +445,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P7"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="75" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="16" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16" style="6" customWidth="1"/>
-    <col min="2" max="12" width="16" style="2"/>
-    <col min="13" max="13" width="16" style="2" customWidth="1"/>
-    <col min="14" max="16384" width="16" style="2"/>
+    <col min="1" max="1" width="16" style="1"/>
+    <col min="2" max="16384" width="16" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="7" t="s">
+    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="B1" s="7"/>
     </row>
-    <row r="2" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+    <row r="4" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+    <row r="5" spans="1:16" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="O6" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="O5" s="5"/>
     </row>
-    <row r="7" spans="1:16" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O7" s="5"/>
-      <c r="P7" s="5"/>
+    <row r="6" spans="1:16" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O6" s="4"/>
+      <c r="P6" s="4"/>
     </row>
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C1:I2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A3:C3"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="62" pageOrder="overThenDown" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="55" orientation="landscape" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddHeader>&amp;L&amp;"IPAPGothic,Regular"【日通システム株式会社】</oddHeader>
+    <oddHeader>&amp;L【日通システム株式会社】</oddHeader>
   </headerFooter>
+  <rowBreaks count="2" manualBreakCount="2">
+    <brk id="65" max="14" man="1"/>
+    <brk id="125" max="16" man="1"/>
+  </rowBreaks>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>